<commit_message>
Basic impl for converting excel to a generic table struct for subsequent processing.
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidrhp/rust/sconv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2A31F6A-150B-8249-8892-8C4CEE691A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4121C3A3-50F5-EC40-A5CA-437B0A4550FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15580" xr2:uid="{FD191831-9341-BF45-805B-B88E93377763}"/>
   </bookViews>
@@ -35,10 +35,53 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>ColumnAfter1</t>
+  </si>
+  <si>
+    <t>Column3</t>
+  </si>
+  <si>
+    <t>Column4</t>
+  </si>
+  <si>
+    <t>2,5</t>
+  </si>
+  <si>
+    <t>four</t>
+  </si>
+  <si>
+    <t>Column5Empty</t>
+  </si>
+  <si>
+    <t>value6Filled</t>
+  </si>
+  <si>
+    <t>fourX</t>
+  </si>
+  <si>
+    <t>value6FilledX</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -66,8 +109,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,14 +428,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD2D87D-74F5-2647-84F1-10232B1D266B}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>20.5</v>
+      </c>
+      <c r="C3">
+        <v>30.5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>